<commit_message>
Deployed 8349aa9 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/uploads/w10/AktivitasDataViz.xlsx
+++ b/uploads/w10/AktivitasDataViz.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kemenkeu-my.sharepoint.com/personal/reza_pratama_kemenkeu_go_id/Documents/Teaching Material/Pengantar TIK/ptik24/docs/uploads/w10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{A5E08013-6E6F-447F-997E-78C3CAB2146E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{030E711C-F30F-4A55-894A-22FC1B059A72}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{A5E08013-6E6F-447F-997E-78C3CAB2146E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D21F182-76C8-4BBF-B932-048FF2359253}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F7660958-6EE9-4387-8E59-370393C7BE76}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{F7660958-6EE9-4387-8E59-370393C7BE76}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruksi" sheetId="7" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -203,6 +203,12 @@
   <si>
     <t>Download/export masing-masing viz menjadi format image (png) - opsional</t>
   </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Rasio</t>
+  </si>
 </sst>
 </file>
 
@@ -273,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -290,6 +296,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4868,8 +4875,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1D60F1D-D155-4483-AC86-297C81D11312}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A17:J31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1D60F1D-D155-4483-AC86-297C81D11312}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A18:J32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField numFmtId="14" showAll="0">
       <items count="244">
@@ -5618,7 +5625,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7CCC1207-CCB2-4AA7-BF79-F2DFDF104EB5}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7CCC1207-CCB2-4AA7-BF79-F2DFDF104EB5}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A6:J20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField numFmtId="14" showAll="0">
@@ -6872,8 +6879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AA58BB-2D8D-45D1-8DCC-D184E20D2458}">
   <dimension ref="A3:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6939,7 +6946,9 @@
   </sheetPr>
   <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -11155,10 +11164,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:J16"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11169,7 +11178,7 @@
     <col min="4" max="4" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" customWidth="1"/>
     <col min="8" max="8" width="8.53125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -11185,7 +11194,7 @@
     <col min="22" max="22" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="8" t="s">
         <v>47</v>
       </c>
@@ -11198,7 +11207,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -11226,8 +11235,32 @@
       <c r="I2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>44562</v>
       </c>
@@ -11255,8 +11288,43 @@
       <c r="I3" s="2">
         <v>13396.600000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="10">
+        <f>B32/B15</f>
+        <v>1.3795954419682861</v>
+      </c>
+      <c r="M3" s="10">
+        <f t="shared" ref="M3:S3" si="0">C32/C15</f>
+        <v>1.1203019304976829</v>
+      </c>
+      <c r="N3" s="10">
+        <f t="shared" si="0"/>
+        <v>1.6596678259228836</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0862792542277884</v>
+      </c>
+      <c r="P3" s="10">
+        <f t="shared" si="0"/>
+        <v>2.0746321634876987</v>
+      </c>
+      <c r="Q3" s="10">
+        <f t="shared" si="0"/>
+        <v>1.3187089097978879</v>
+      </c>
+      <c r="R3" s="10">
+        <f t="shared" si="0"/>
+        <v>1.5985686379666941</v>
+      </c>
+      <c r="S3" s="10">
+        <f t="shared" si="0"/>
+        <v>1.5533824943541865</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>44593</v>
       </c>
@@ -11285,7 +11353,7 @@
         <v>12726.770000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>44621</v>
       </c>
@@ -11314,7 +11382,7 @@
         <v>25118.625000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>44652</v>
       </c>
@@ -11343,7 +11411,7 @@
         <v>14736.260000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>44682</v>
       </c>
@@ -11372,7 +11440,7 @@
         <v>22439.305000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>44713</v>
       </c>
@@ -11401,7 +11469,7 @@
         <v>25788.455000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>44743</v>
       </c>
@@ -11430,7 +11498,7 @@
         <v>20429.815000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>44774</v>
       </c>
@@ -11459,7 +11527,7 @@
         <v>10047.450000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>44805</v>
       </c>
@@ -11488,7 +11556,7 @@
         <v>26123.370000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>44835</v>
       </c>
@@ -11517,7 +11585,7 @@
         <v>16410.835000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>44866</v>
       </c>
@@ -11546,7 +11614,7 @@
         <v>24783.710000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>44896</v>
       </c>
@@ -11575,485 +11643,522 @@
         <v>16745.750000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="A16" s="9" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2">
+        <f>SUM(B3:B14)</f>
+        <v>251856.08</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" ref="C15:I15" si="1">SUM(C3:C14)</f>
+        <v>254535.40000000008</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>206642.55500000005</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>212001.19500000007</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>233100.84000000003</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>207982.21500000005</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>222048.64500000002</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>228746.94500000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.75">
+      <c r="A17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>7</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>4</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>5</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>6</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J19" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>33491.500000000007</v>
-      </c>
-      <c r="C19">
-        <v>25992</v>
-      </c>
-      <c r="D19">
-        <v>41489</v>
-      </c>
-      <c r="E19">
-        <v>10065</v>
-      </c>
-      <c r="F19">
-        <v>29370</v>
-      </c>
-      <c r="G19">
-        <v>3840</v>
-      </c>
-      <c r="H19">
-        <v>46815.5</v>
-      </c>
-      <c r="I19">
-        <v>32934</v>
-      </c>
-      <c r="J19">
-        <v>223997</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20">
-        <v>18487</v>
+        <v>33491.500000000007</v>
       </c>
       <c r="C20">
-        <v>26712</v>
+        <v>25992</v>
       </c>
       <c r="D20">
-        <v>44712.5</v>
+        <v>41489</v>
       </c>
       <c r="E20">
-        <v>25735.5</v>
+        <v>10065</v>
       </c>
       <c r="F20">
-        <v>40473</v>
+        <v>29370</v>
       </c>
       <c r="G20">
-        <v>13747.5</v>
+        <v>3840</v>
       </c>
       <c r="H20">
-        <v>13608</v>
+        <v>46815.5</v>
       </c>
       <c r="I20">
-        <v>30594</v>
+        <v>32934</v>
       </c>
       <c r="J20">
-        <v>214069.5</v>
+        <v>223997</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21">
-        <v>36937.5</v>
+        <v>18487</v>
       </c>
       <c r="C21">
-        <v>10752</v>
+        <v>26712</v>
       </c>
       <c r="D21">
-        <v>36432</v>
+        <v>44712.5</v>
       </c>
       <c r="E21">
-        <v>2709</v>
+        <v>25735.5</v>
       </c>
       <c r="F21">
-        <v>24065</v>
+        <v>40473</v>
       </c>
       <c r="G21">
-        <v>42611</v>
+        <v>13747.5</v>
       </c>
       <c r="H21">
-        <v>51468</v>
+        <v>13608</v>
       </c>
       <c r="I21">
-        <v>2436</v>
+        <v>30594</v>
       </c>
       <c r="J21">
-        <v>207410.5</v>
+        <v>214069.5</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22">
-        <v>9768</v>
+        <v>36937.5</v>
       </c>
       <c r="C22">
-        <v>27659</v>
+        <v>10752</v>
       </c>
       <c r="D22">
-        <v>12960</v>
+        <v>36432</v>
       </c>
       <c r="E22">
-        <v>20778.5</v>
+        <v>2709</v>
       </c>
       <c r="F22">
-        <v>44425</v>
+        <v>24065</v>
       </c>
       <c r="G22">
-        <v>53449</v>
+        <v>42611</v>
       </c>
       <c r="H22">
-        <v>20119</v>
+        <v>51468</v>
       </c>
       <c r="I22">
-        <v>48411.5</v>
+        <v>2436</v>
       </c>
       <c r="J22">
-        <v>237570</v>
+        <v>207410.5</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
-        <v>28815</v>
+        <v>9768</v>
       </c>
       <c r="C23">
-        <v>36517</v>
+        <v>27659</v>
       </c>
       <c r="D23">
-        <v>44604</v>
+        <v>12960</v>
       </c>
       <c r="E23">
-        <v>23310</v>
+        <v>20778.5</v>
       </c>
       <c r="F23">
-        <v>8680</v>
+        <v>44425</v>
       </c>
       <c r="G23">
-        <v>25804</v>
+        <v>53449</v>
       </c>
       <c r="H23">
-        <v>38477</v>
+        <v>20119</v>
       </c>
       <c r="I23">
-        <v>18209.5</v>
+        <v>48411.5</v>
       </c>
       <c r="J23">
-        <v>224416.5</v>
+        <v>237570</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
-        <v>19036.500000000004</v>
+        <v>28815</v>
       </c>
       <c r="C24">
-        <v>37274.5</v>
+        <v>36517</v>
       </c>
       <c r="D24">
-        <v>15938</v>
+        <v>44604</v>
       </c>
       <c r="E24">
-        <v>23194.5</v>
+        <v>23310</v>
       </c>
       <c r="F24">
-        <v>57987.5</v>
+        <v>8680</v>
       </c>
       <c r="G24">
-        <v>18229.5</v>
+        <v>25804</v>
       </c>
       <c r="H24">
-        <v>46295</v>
+        <v>38477</v>
       </c>
       <c r="I24">
-        <v>13809</v>
+        <v>18209.5</v>
       </c>
       <c r="J24">
-        <v>231764.5</v>
+        <v>224416.5</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
-        <v>38506.5</v>
+        <v>19036.500000000004</v>
       </c>
       <c r="C25">
-        <v>32064.5</v>
+        <v>37274.5</v>
       </c>
       <c r="D25">
-        <v>36759.5</v>
+        <v>15938</v>
       </c>
       <c r="E25">
-        <v>28212</v>
+        <v>23194.5</v>
       </c>
       <c r="F25">
-        <v>34731</v>
+        <v>57987.5</v>
       </c>
       <c r="G25">
-        <v>14736</v>
+        <v>18229.5</v>
       </c>
       <c r="H25">
-        <v>35333.5</v>
+        <v>46295</v>
       </c>
       <c r="I25">
-        <v>12820.5</v>
+        <v>13809</v>
       </c>
       <c r="J25">
-        <v>233163.5</v>
+        <v>231764.5</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
-        <v>39775.5</v>
+        <v>38506.5</v>
       </c>
       <c r="C26">
-        <v>21105</v>
+        <v>32064.5</v>
       </c>
       <c r="D26">
-        <v>12691</v>
+        <v>36759.5</v>
       </c>
       <c r="E26">
-        <v>7308</v>
+        <v>28212</v>
       </c>
       <c r="F26">
-        <v>52870.5</v>
+        <v>34731</v>
       </c>
       <c r="G26">
-        <v>38063</v>
+        <v>14736</v>
+      </c>
+      <c r="H26">
+        <v>35333.5</v>
       </c>
       <c r="I26">
-        <v>34951.5</v>
+        <v>12820.5</v>
       </c>
       <c r="J26">
-        <v>206764.5</v>
+        <v>233163.5</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
-        <v>58117</v>
+        <v>39775.5</v>
       </c>
       <c r="C27">
-        <v>27755</v>
+        <v>21105</v>
       </c>
       <c r="D27">
-        <v>14175.000000000002</v>
+        <v>12691</v>
       </c>
       <c r="E27">
-        <v>34737.5</v>
+        <v>7308</v>
       </c>
       <c r="F27">
-        <v>34975</v>
+        <v>52870.5</v>
       </c>
       <c r="G27">
-        <v>26190.500000000004</v>
-      </c>
-      <c r="H27">
-        <v>28302</v>
+        <v>38063</v>
       </c>
       <c r="I27">
-        <v>17375.000000000004</v>
+        <v>34951.5</v>
       </c>
       <c r="J27">
-        <v>241627</v>
+        <v>206764.5</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
-        <v>16625</v>
+        <v>58117</v>
       </c>
       <c r="C28">
-        <v>25210.5</v>
+        <v>27755</v>
       </c>
       <c r="D28">
-        <v>17260</v>
+        <v>14175.000000000002</v>
       </c>
       <c r="E28">
-        <v>12120</v>
+        <v>34737.5</v>
       </c>
       <c r="F28">
-        <v>60431</v>
+        <v>34975</v>
       </c>
       <c r="G28">
-        <v>29455.5</v>
+        <v>26190.500000000004</v>
       </c>
       <c r="H28">
-        <v>18270</v>
+        <v>28302</v>
       </c>
       <c r="I28">
-        <v>43726</v>
+        <v>17375.000000000004</v>
       </c>
       <c r="J28">
-        <v>223098</v>
+        <v>241627</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29">
-        <v>35210</v>
+        <v>16625</v>
       </c>
       <c r="C29">
-        <v>6080</v>
+        <v>25210.5</v>
       </c>
       <c r="D29">
-        <v>21469.5</v>
+        <v>17260</v>
       </c>
       <c r="E29">
-        <v>29678.5</v>
+        <v>12120</v>
       </c>
       <c r="F29">
-        <v>42553</v>
+        <v>60431</v>
       </c>
       <c r="G29">
-        <v>8142</v>
+        <v>29455.5</v>
       </c>
       <c r="H29">
-        <v>34774.5</v>
+        <v>18270</v>
       </c>
       <c r="I29">
-        <v>80327</v>
+        <v>43726</v>
       </c>
       <c r="J29">
-        <v>258234.5</v>
+        <v>223098</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30">
-        <v>12690</v>
+        <v>35210</v>
       </c>
       <c r="C30">
-        <v>8035</v>
+        <v>6080</v>
       </c>
       <c r="D30">
-        <v>44467.5</v>
+        <v>21469.5</v>
       </c>
       <c r="E30">
-        <v>12444</v>
+        <v>29678.5</v>
       </c>
       <c r="F30">
-        <v>53037.5</v>
+        <v>42553</v>
+      </c>
+      <c r="G30">
+        <v>8142</v>
       </c>
       <c r="H30">
-        <v>21497.5</v>
+        <v>34774.5</v>
       </c>
       <c r="I30">
-        <v>19737.5</v>
+        <v>80327</v>
       </c>
       <c r="J30">
-        <v>171909</v>
+        <v>258234.5</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>12690</v>
+      </c>
+      <c r="C31">
+        <v>8035</v>
+      </c>
+      <c r="D31">
+        <v>44467.5</v>
+      </c>
+      <c r="E31">
+        <v>12444</v>
+      </c>
+      <c r="F31">
+        <v>53037.5</v>
+      </c>
+      <c r="H31">
+        <v>21497.5</v>
+      </c>
+      <c r="I31">
+        <v>19737.5</v>
+      </c>
+      <c r="J31">
+        <v>171909</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>347459.5</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>285156.5</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>342958</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>230292.5</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>483598.5</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>274268</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>354960</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <v>355331.5</v>
       </c>
-      <c r="J31">
+      <c r="J32">
         <v>2674024.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12063,8 +12168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B684AEC9-5259-4364-BB4D-AED471068E02}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12472,7 +12577,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>